<commit_message>
[CHILI GraFx] Multichannel nuances (#323)
</commit_message>
<xml_diff>
--- a/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
+++ b/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bram/Documents/GitHub/grafx-documentation/docs/CHILI-GraFx/applications/editor-comparison/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bram/Documents/GitHub.nosync/grafx-documentation/docs/CHILI-GraFx/applications/editor-comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80F61E0-EDEB-3749-9E6B-E52861C30C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF7FB14-B629-1041-9536-4B63F9E22470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9760" yWindow="760" windowWidth="20480" windowHeight="18880" xr2:uid="{BF9F8A34-DC7E-0549-A389-ADCA54F02979}"/>
   </bookViews>
@@ -584,9 +584,6 @@
     <t>❇️</t>
   </si>
   <si>
-    <t xml:space="preserve"> ❇️ By end of 2023</t>
-  </si>
-  <si>
     <t>Replaced by connector framework in GraFx Studio</t>
   </si>
   <si>
@@ -612,6 +609,9 @@
   </si>
   <si>
     <t>GraFx Studio: via API</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ❇️ Being developped</t>
   </si>
 </sst>
 </file>
@@ -680,9 +680,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -720,7 +720,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -826,7 +826,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -968,7 +968,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -978,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26496501-D774-604E-8805-246C457AC686}">
   <dimension ref="A1:D175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D164" sqref="D164"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,7 +1009,7 @@
         <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>131</v>
@@ -1065,7 +1065,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>128</v>
@@ -1177,7 +1177,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>128</v>
@@ -1289,7 +1289,7 @@
         <v>176</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>128</v>
@@ -1303,7 +1303,7 @@
         <v>177</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>128</v>
@@ -1779,7 +1779,7 @@
         <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>128</v>
@@ -1799,7 +1799,7 @@
         <v>128</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1841,7 +1841,7 @@
         <v>128</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1849,7 +1849,7 @@
         <v>175</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>128</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>128</v>
@@ -2031,7 +2031,7 @@
         <v>50</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>128</v>
@@ -2157,7 +2157,7 @@
         <v>58</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>128</v>
@@ -2171,7 +2171,7 @@
         <v>59</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>128</v>
@@ -2185,7 +2185,7 @@
         <v>60</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>128</v>
@@ -2227,7 +2227,7 @@
         <v>63</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>128</v>
@@ -2241,7 +2241,7 @@
         <v>64</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>128</v>
@@ -2255,7 +2255,7 @@
         <v>65</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>128</v>
@@ -2297,7 +2297,7 @@
         <v>67</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>128</v>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>128</v>
@@ -2535,7 +2535,7 @@
         <v>159</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>128</v>
@@ -2549,7 +2549,7 @@
         <v>158</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>128</v>
@@ -2563,7 +2563,7 @@
         <v>157</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>128</v>
@@ -2605,7 +2605,7 @@
         <v>161</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>128</v>
@@ -2633,7 +2633,7 @@
         <v>163</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>128</v>
@@ -2871,7 +2871,7 @@
         <v>90</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>128</v>
@@ -2896,7 +2896,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>128</v>
@@ -3078,7 +3078,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>128</v>
@@ -3092,7 +3092,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>128</v>
@@ -3120,7 +3120,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>131</v>
@@ -3235,7 +3235,7 @@
         <v>107</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>128</v>
@@ -3249,7 +3249,7 @@
         <v>108</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>128</v>
@@ -3260,10 +3260,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>128</v>
@@ -3283,7 +3283,7 @@
         <v>128</v>
       </c>
       <c r="D164" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update xls with comparison
</commit_message>
<xml_diff>
--- a/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
+++ b/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bram/Documents/GitHub.nosync/grafx-documentation/docs/CHILI-GraFx/applications/editor-comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF7FB14-B629-1041-9536-4B63F9E22470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412CC5CA-325E-F44F-A7DC-BD989B0836AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9760" yWindow="760" windowWidth="20480" windowHeight="18880" xr2:uid="{BF9F8A34-DC7E-0549-A389-ADCA54F02979}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="29920" windowHeight="18580" xr2:uid="{BF9F8A34-DC7E-0549-A389-ADCA54F02979}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="208">
   <si>
     <t>Feature</t>
   </si>
@@ -209,9 +209,6 @@
     <t xml:space="preserve">Custom color swatches </t>
   </si>
   <si>
-    <t xml:space="preserve">Pre-defined barcode setup in backoffice </t>
-  </si>
-  <si>
     <t xml:space="preserve">Support for datamatrix </t>
   </si>
   <si>
@@ -443,9 +440,6 @@
     <t>Layouts</t>
   </si>
   <si>
-    <t>GraFx Studio supports inheritance in layouts</t>
-  </si>
-  <si>
     <t>GraFx Studio supports JavaScript based Actions</t>
   </si>
   <si>
@@ -551,18 +545,9 @@
     <t>**Text Editing**</t>
   </si>
   <si>
-    <t>Support for external URL (xml feed)</t>
-  </si>
-  <si>
     <t>Support for dynamic asset providers</t>
   </si>
   <si>
-    <t>Through connector framework in GraFx Studio</t>
-  </si>
-  <si>
-    <t>GraFx Studio: Combination of hidden fields and Actions</t>
-  </si>
-  <si>
     <t xml:space="preserve">Automatic Cropping </t>
   </si>
   <si>
@@ -584,9 +569,6 @@
     <t>❇️</t>
   </si>
   <si>
-    <t>Replaced by connector framework in GraFx Studio</t>
-  </si>
-  <si>
     <t>Define rotation</t>
   </si>
   <si>
@@ -608,10 +590,76 @@
     <t xml:space="preserve">Frame positioning, resizing and rotation based on variables </t>
   </si>
   <si>
-    <t>GraFx Studio: via API</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ❇️ Being developped</t>
+  </si>
+  <si>
+    <t>See Connector Framework</t>
+  </si>
+  <si>
+    <t>Pre-defined barcodes</t>
+  </si>
+  <si>
+    <t>GraFx Studio through Connectors</t>
+  </si>
+  <si>
+    <t>GraFx Genie (AI assistent for Actions)</t>
+  </si>
+  <si>
+    <t>Inheritance model for layouts</t>
+  </si>
+  <si>
+    <t>Layout intents defined per layout</t>
+  </si>
+  <si>
+    <t>Through connector Hub in GraFx Studio</t>
+  </si>
+  <si>
+    <t>Support for Code 39</t>
+  </si>
+  <si>
+    <t>Support for Code 93</t>
+  </si>
+  <si>
+    <t>Support for EAN8</t>
+  </si>
+  <si>
+    <t>Support for UPC-A</t>
+  </si>
+  <si>
+    <t>Support for UPC-E</t>
+  </si>
+  <si>
+    <t>Support for Code 128</t>
+  </si>
+  <si>
+    <t>Stylekits</t>
+  </si>
+  <si>
+    <t>Support for metadata mapping from DAM</t>
+  </si>
+  <si>
+    <t>GraFx Studio: Support via JavaScript actions</t>
+  </si>
+  <si>
+    <t>**Self-serve**</t>
+  </si>
+  <si>
+    <t>Support for Out-of-the-box self service</t>
+  </si>
+  <si>
+    <t>GraFx Studio: My Projects</t>
+  </si>
+  <si>
+    <t>Support for Collections</t>
+  </si>
+  <si>
+    <t>Support for Font Families</t>
+  </si>
+  <si>
+    <t>Support for Font Styles</t>
+  </si>
+  <si>
+    <t>Connector Framework</t>
   </si>
 </sst>
 </file>
@@ -976,16 +1024,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26496501-D774-604E-8805-246C457AC686}">
-  <dimension ref="A1:D175"/>
+  <dimension ref="A1:D191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52.5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
   </cols>
@@ -995,136 +1043,136 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>201</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>202</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>131</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>204</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -1132,13 +1180,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>1</v>
@@ -1146,13 +1194,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>1</v>
@@ -1160,13 +1208,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1</v>
@@ -1174,13 +1222,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
@@ -1188,13 +1236,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -1202,13 +1250,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1</v>
@@ -1216,13 +1264,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>128</v>
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -1230,13 +1278,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>169</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>128</v>
+        <v>198</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
@@ -1244,153 +1292,153 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>128</v>
+        <v>13</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>176</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>128</v>
+        <v>167</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>177</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>178</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>131</v>
+        <v>16</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>179</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>128</v>
+        <v>17</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>128</v>
+        <v>171</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>172</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>128</v>
+        <v>173</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>1</v>
+        <v>174</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>1</v>
@@ -1398,27 +1446,27 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>128</v>
+        <v>18</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>180</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>1</v>
@@ -1426,13 +1474,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>128</v>
+        <v>20</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>1</v>
@@ -1440,13 +1488,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>1</v>
@@ -1454,27 +1502,27 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>1</v>
@@ -1482,13 +1530,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>1</v>
@@ -1496,13 +1544,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>1</v>
@@ -1510,13 +1558,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>1</v>
@@ -1524,13 +1572,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>1</v>
@@ -1538,13 +1586,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>1</v>
@@ -1552,13 +1600,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>1</v>
@@ -1566,13 +1614,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>1</v>
@@ -1580,13 +1628,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>1</v>
@@ -1594,13 +1642,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>1</v>
@@ -1608,13 +1656,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>1</v>
@@ -1622,27 +1670,27 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>1</v>
@@ -1650,13 +1698,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>205</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>1</v>
@@ -1664,13 +1712,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>206</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>1</v>
@@ -1678,13 +1726,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>1</v>
@@ -1692,13 +1740,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>128</v>
+        <v>36</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>1</v>
@@ -1706,27 +1754,27 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>128</v>
+        <v>37</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>128</v>
+        <v>38</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>1</v>
@@ -1734,13 +1782,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>128</v>
+        <v>39</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>1</v>
@@ -1748,13 +1796,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>181</v>
+        <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>1</v>
@@ -1762,13 +1810,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>46</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>128</v>
+        <v>115</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>1</v>
@@ -1776,13 +1824,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>47</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>128</v>
+        <v>41</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>1</v>
@@ -1790,27 +1838,27 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>171</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>181</v>
+        <v>42</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>182</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>48</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>1</v>
@@ -1818,13 +1866,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>49</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>181</v>
+        <v>44</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>1</v>
@@ -1832,27 +1880,27 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>172</v>
+        <v>45</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>182</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>175</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>181</v>
+        <v>46</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>1</v>
@@ -1860,13 +1908,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>1</v>
@@ -1874,13 +1922,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>143</v>
+        <v>207</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>1</v>
@@ -1888,13 +1936,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>144</v>
+        <v>48</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>1</v>
@@ -1902,13 +1950,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>145</v>
+        <v>49</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>1</v>
@@ -1916,27 +1964,27 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>1</v>
@@ -1944,10 +1992,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>1</v>
@@ -1958,10 +2006,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>1</v>
@@ -1972,10 +2020,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>1</v>
@@ -1986,10 +2034,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>1</v>
@@ -2000,10 +2048,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>151</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>1</v>
@@ -2014,10 +2062,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>1</v>
@@ -2028,13 +2076,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>50</v>
+        <v>146</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>1</v>
@@ -2042,13 +2090,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>1</v>
@@ -2056,13 +2104,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>52</v>
+        <v>177</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>1</v>
@@ -2070,13 +2118,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>53</v>
+        <v>148</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>1</v>
@@ -2084,13 +2132,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>54</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>1</v>
+        <v>149</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>1</v>
@@ -2098,13 +2146,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>1</v>
@@ -2112,13 +2160,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>1</v>
@@ -2126,13 +2174,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>1</v>
@@ -2140,13 +2188,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>1</v>
@@ -2154,13 +2202,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>181</v>
+        <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>1</v>
@@ -2168,13 +2216,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>1</v>
@@ -2182,13 +2230,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>181</v>
+        <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>1</v>
@@ -2196,13 +2244,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>1</v>
@@ -2210,13 +2258,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>1</v>
@@ -2224,13 +2272,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>63</v>
+        <v>186</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>1</v>
@@ -2238,13 +2286,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>64</v>
+        <v>192</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>1</v>
@@ -2252,13 +2300,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>1</v>
@@ -2266,13 +2314,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>66</v>
+        <v>197</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>1</v>
@@ -2280,13 +2328,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>119</v>
+        <v>57</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>1</v>
@@ -2294,13 +2342,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>67</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>181</v>
+        <v>195</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>1</v>
@@ -2308,10 +2356,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>120</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>1</v>
@@ -2322,13 +2370,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>68</v>
+        <v>196</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>1</v>
@@ -2336,13 +2384,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>1</v>
@@ -2350,13 +2398,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>70</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>1</v>
+        <v>194</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>1</v>
@@ -2364,13 +2412,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>1</v>
@@ -2378,13 +2426,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>181</v>
+        <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>1</v>
@@ -2392,13 +2440,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>1</v>
@@ -2406,13 +2454,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>1</v>
@@ -2420,13 +2468,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>1</v>
@@ -2434,13 +2482,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>1</v>
@@ -2448,13 +2496,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>1</v>
@@ -2462,13 +2510,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>1</v>
@@ -2476,13 +2524,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>181</v>
+        <v>1</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>1</v>
@@ -2490,13 +2538,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>121</v>
+        <v>67</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>1</v>
@@ -2504,13 +2552,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>184</v>
+        <v>68</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>1</v>
@@ -2518,13 +2566,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>155</v>
+        <v>69</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>1</v>
@@ -2532,13 +2580,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>159</v>
+        <v>70</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>181</v>
+        <v>1</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>1</v>
@@ -2546,13 +2594,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>158</v>
+        <v>71</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>1</v>
@@ -2560,13 +2608,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>157</v>
+        <v>72</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>1</v>
@@ -2574,27 +2622,27 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>156</v>
+        <v>73</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>174</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>160</v>
+        <v>74</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>1</v>
@@ -2602,13 +2650,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>161</v>
+        <v>75</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>181</v>
+        <v>1</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>1</v>
@@ -2616,13 +2664,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>1</v>
@@ -2630,13 +2678,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>163</v>
+        <v>77</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>181</v>
+        <v>1</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>1</v>
@@ -2644,13 +2692,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>164</v>
+        <v>78</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>1</v>
@@ -2658,13 +2706,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>165</v>
+        <v>120</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>1</v>
@@ -2672,13 +2720,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>1</v>
@@ -2686,13 +2734,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>1</v>
@@ -2700,13 +2748,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>1</v>
@@ -2714,13 +2762,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>1</v>
@@ -2728,13 +2776,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>81</v>
+        <v>155</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>1</v>
@@ -2742,27 +2790,27 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>82</v>
+        <v>154</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>83</v>
+        <v>158</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>1</v>
@@ -2770,13 +2818,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>1</v>
@@ -2784,13 +2832,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>1</v>
@@ -2798,13 +2846,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>86</v>
+        <v>161</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>1</v>
@@ -2812,13 +2860,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>1</v>
@@ -2826,13 +2874,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>122</v>
+        <v>163</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>1</v>
@@ -2840,13 +2888,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>88</v>
+        <v>164</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>1</v>
@@ -2854,13 +2902,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>1</v>
@@ -2868,13 +2916,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>181</v>
+        <v>1</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>1</v>
@@ -2882,13 +2930,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>1</v>
@@ -2896,27 +2944,27 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>185</v>
+        <v>80</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>1</v>
@@ -2924,13 +2972,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>1</v>
@@ -2938,41 +2986,41 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>132</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>128</v>
+        <v>83</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>134</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>128</v>
+        <v>84</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>135</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>94</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>128</v>
+        <v>85</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>1</v>
@@ -2980,13 +3028,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>1</v>
@@ -2994,27 +3042,27 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>96</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>136</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>97</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>128</v>
+        <v>87</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>1</v>
@@ -3022,13 +3070,13 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>98</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>128</v>
+        <v>88</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>1</v>
@@ -3036,13 +3084,13 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>1</v>
@@ -3050,13 +3098,13 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>1</v>
@@ -3064,94 +3112,94 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>100</v>
+        <v>179</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>189</v>
+        <v>91</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>137</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>186</v>
+        <v>92</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>137</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>101</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>187</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>102</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>128</v>
+        <v>189</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>173</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>124</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>1</v>
+        <v>190</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>1</v>
@@ -3162,13 +3210,13 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>103</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>181</v>
+        <v>93</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>1</v>
@@ -3176,13 +3224,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>181</v>
+        <v>1</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>1</v>
@@ -3190,27 +3238,27 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>105</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>181</v>
+        <v>95</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1</v>
+        <v>134</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>125</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>1</v>
+        <v>96</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>1</v>
@@ -3218,13 +3266,13 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>106</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>1</v>
@@ -3232,13 +3280,13 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>107</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>1</v>
@@ -3246,27 +3294,27 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>138</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>1</v>
@@ -3274,97 +3322,97 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D164" t="s">
-        <v>190</v>
+        <v>127</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>152</v>
+        <v>183</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>1</v>
+        <v>135</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>1</v>
+        <v>135</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>154</v>
+        <v>100</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>1</v>
+        <v>135</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>1</v>
+        <v>191</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>139</v>
+        <v>199</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>1</v>
@@ -3372,7 +3420,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>1</v>
@@ -3386,27 +3434,27 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>1</v>
+        <v>187</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>1</v>
@@ -3414,13 +3462,13 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>1</v>
@@ -3428,15 +3476,239 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="D175" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>105</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>106</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>107</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>182</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>108</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>150</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>151</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>152</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>138</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>109</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>137</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>125</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>110</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>139</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>111</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>112</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D191" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[GraFx Studio] Feature Comparison (#418)
</commit_message>
<xml_diff>
--- a/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
+++ b/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bram/Documents/GitHub.nosync/grafx-documentation/docs/CHILI-GraFx/applications/editor-comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF7FB14-B629-1041-9536-4B63F9E22470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5EB5E9-162D-DD4E-9C99-A5A20702AFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9760" yWindow="760" windowWidth="20480" windowHeight="18880" xr2:uid="{BF9F8A34-DC7E-0549-A389-ADCA54F02979}"/>
+    <workbookView xWindow="9960" yWindow="760" windowWidth="28440" windowHeight="20840" xr2:uid="{BF9F8A34-DC7E-0549-A389-ADCA54F02979}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="192">
-  <si>
-    <t>Feature</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="194">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -71,15 +68,9 @@
     <t xml:space="preserve">Support for annotations </t>
   </si>
   <si>
-    <t xml:space="preserve">Support for document rotation </t>
-  </si>
-  <si>
     <t xml:space="preserve">Configurable Asset directories </t>
   </si>
   <si>
-    <t xml:space="preserve">Advanced border and fill settings </t>
-  </si>
-  <si>
     <t xml:space="preserve">Transparency  </t>
   </si>
   <si>
@@ -113,9 +104,6 @@
     <t xml:space="preserve">Paste text copied from clipboard </t>
   </si>
   <si>
-    <t xml:space="preserve">Edit text in non-orthogonal frame </t>
-  </si>
-  <si>
     <t xml:space="preserve">Edit text along path </t>
   </si>
   <si>
@@ -134,9 +122,6 @@
     <t xml:space="preserve">Text wrapping around other objects </t>
   </si>
   <si>
-    <t xml:space="preserve">Text wrapping around non orthogonal shapes </t>
-  </si>
-  <si>
     <t xml:space="preserve">Support for TrueType fonts </t>
   </si>
   <si>
@@ -170,18 +155,12 @@
     <t xml:space="preserve">Automatic Image fitting </t>
   </si>
   <si>
-    <t xml:space="preserve">Different image selection methods </t>
-  </si>
-  <si>
     <t xml:space="preserve">Upload images from local client </t>
   </si>
   <si>
     <t xml:space="preserve">Basic image repository </t>
   </si>
   <si>
-    <t xml:space="preserve">Link to external image repositories </t>
-  </si>
-  <si>
     <t xml:space="preserve">Support for image transformations </t>
   </si>
   <si>
@@ -209,15 +188,6 @@
     <t xml:space="preserve">Custom color swatches </t>
   </si>
   <si>
-    <t xml:space="preserve">Pre-defined barcode setup in backoffice </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Support for datamatrix </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Support for UPC </t>
-  </si>
-  <si>
     <t xml:space="preserve">Support for EAN13 </t>
   </si>
   <si>
@@ -227,24 +197,9 @@
     <t xml:space="preserve">Support for ISBN </t>
   </si>
   <si>
-    <t xml:space="preserve">GS1-128 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS1-Datamatrix </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDF417 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pharmacode 1-bar </t>
-  </si>
-  <si>
     <t xml:space="preserve">Configurable preflight warnings and errors, including text overflow and resolution </t>
   </si>
   <si>
-    <t xml:space="preserve">Selectively lock, unlock or allow specific edits on frames </t>
-  </si>
-  <si>
     <t xml:space="preserve">Document constraints </t>
   </si>
   <si>
@@ -260,24 +215,6 @@
     <t xml:space="preserve">Frame content constraints </t>
   </si>
   <si>
-    <t xml:space="preserve">Pre-defined constraints (apply to multiple documents) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limit styles for specific frames </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limit font usage per document </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limit font usage per text frame </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move region </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Granular constraints (frame, layer, document) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Use variables in text frames  </t>
   </si>
   <si>
@@ -302,9 +239,6 @@
     <t xml:space="preserve">Create variables in document </t>
   </si>
   <si>
-    <t xml:space="preserve">Make templates smart so they can react to changes in content </t>
-  </si>
-  <si>
     <t xml:space="preserve">Automate Artwork Production </t>
   </si>
   <si>
@@ -314,12 +248,6 @@
     <t xml:space="preserve">Copyfitting of text in variables </t>
   </si>
   <si>
-    <t xml:space="preserve">Copyfitting across multiple frames </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apply copyfitting on individual frames </t>
-  </si>
-  <si>
     <t xml:space="preserve">Support for multiple output dimensions </t>
   </si>
   <si>
@@ -356,12 +284,6 @@
     <t xml:space="preserve">Support for structured files (csv, excel, xml) </t>
   </si>
   <si>
-    <t xml:space="preserve">Text overflow preflight warning </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDF Standards </t>
-  </si>
-  <si>
     <t xml:space="preserve">Output to PDF  </t>
   </si>
   <si>
@@ -437,27 +359,15 @@
     <t>Anchoring</t>
   </si>
   <si>
-    <t>In GraFx Studio through Actions</t>
-  </si>
-  <si>
     <t>Layouts</t>
   </si>
   <si>
-    <t>GraFx Studio supports inheritance in layouts</t>
-  </si>
-  <si>
     <t>GraFx Studio supports JavaScript based Actions</t>
   </si>
   <si>
     <t>GraFx Studio through Actions</t>
   </si>
   <si>
-    <t>GraFx Studio: no presets yet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output to Adobe InDesign (IDML) </t>
-  </si>
-  <si>
     <t>Output to MP4</t>
   </si>
   <si>
@@ -488,9 +398,6 @@
     <t>Define ease type</t>
   </si>
   <si>
-    <t>Define scaling</t>
-  </si>
-  <si>
     <t>Maintain animation across layouts</t>
   </si>
   <si>
@@ -539,9 +446,6 @@
     <t>Type: Coordinate</t>
   </si>
   <si>
-    <t>Type: Divider</t>
-  </si>
-  <si>
     <t>Type: Button Bar</t>
   </si>
   <si>
@@ -551,21 +455,9 @@
     <t>**Text Editing**</t>
   </si>
   <si>
-    <t>Support for external URL (xml feed)</t>
-  </si>
-  <si>
     <t>Support for dynamic asset providers</t>
   </si>
   <si>
-    <t>Through connector framework in GraFx Studio</t>
-  </si>
-  <si>
-    <t>GraFx Studio: Combination of hidden fields and Actions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automatic Cropping </t>
-  </si>
-  <si>
     <t>Frame Positioning: mm</t>
   </si>
   <si>
@@ -578,18 +470,9 @@
     <t>Frame Positioning: pixels (px)</t>
   </si>
   <si>
-    <t>GraFx Studio: only for Template Designers</t>
-  </si>
-  <si>
     <t>❇️</t>
   </si>
   <si>
-    <t>Replaced by connector framework in GraFx Studio</t>
-  </si>
-  <si>
-    <t>Define rotation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Use variables to insert content into templates </t>
   </si>
   <si>
@@ -602,16 +485,139 @@
     <t>**External Assets**</t>
   </si>
   <si>
-    <t xml:space="preserve">Output to PDF with crop and/or bleed marks </t>
-  </si>
-  <si>
     <t xml:space="preserve">Frame positioning, resizing and rotation based on variables </t>
   </si>
   <si>
-    <t>GraFx Studio: via API</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ❇️ Being developped</t>
+    <t>Pre-defined barcodes</t>
+  </si>
+  <si>
+    <t>Inheritance model for layouts</t>
+  </si>
+  <si>
+    <t>Layout intents defined per layout</t>
+  </si>
+  <si>
+    <t>Support for Code 39</t>
+  </si>
+  <si>
+    <t>Support for EAN8</t>
+  </si>
+  <si>
+    <t>Support for UPC-A</t>
+  </si>
+  <si>
+    <t>Support for UPC-E</t>
+  </si>
+  <si>
+    <t>Support for Code 128</t>
+  </si>
+  <si>
+    <t>Support for metadata mapping from DAM</t>
+  </si>
+  <si>
+    <t>GraFx Studio: Support via JavaScript actions</t>
+  </si>
+  <si>
+    <t>**Self-serve**</t>
+  </si>
+  <si>
+    <t>Support for Out-of-the-box self service</t>
+  </si>
+  <si>
+    <t>GraFx Studio: My Projects</t>
+  </si>
+  <si>
+    <t>Connector Framework</t>
+  </si>
+  <si>
+    <t>Feature / Capability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output to IDML </t>
+  </si>
+  <si>
+    <t>**Input**</t>
+  </si>
+  <si>
+    <t>Import from Adobe® InDesign®</t>
+  </si>
+  <si>
+    <t>Import from Adobe® PhotoShop®</t>
+  </si>
+  <si>
+    <t>**Batch Processing**</t>
+  </si>
+  <si>
+    <t>Batch processing of records</t>
+  </si>
+  <si>
+    <t>Baseline shift</t>
+  </si>
+  <si>
+    <t>GraFx Studio: Through Media Connectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Border and fill settings </t>
+  </si>
+  <si>
+    <t>GraFx Studio: in Template Designer Workspace</t>
+  </si>
+  <si>
+    <t>Support for Font Families management</t>
+  </si>
+  <si>
+    <t>Support for Font Styles management</t>
+  </si>
+  <si>
+    <t>Link to external image repositories (e.g. DAM)</t>
+  </si>
+  <si>
+    <t>AI powered Smart Crop</t>
+  </si>
+  <si>
+    <t>Define tween type</t>
+  </si>
+  <si>
+    <t>Support for Code 39 Extended</t>
+  </si>
+  <si>
+    <t>Support for ITF14</t>
+  </si>
+  <si>
+    <t>Support for Code 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Support for DataMatrix </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Support for GS1-128 </t>
+  </si>
+  <si>
+    <t>Support for GS1-Databar Expanded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Support for PDF417 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Support for Pharmacode 1-bar </t>
+  </si>
+  <si>
+    <t>Support for Postnet</t>
+  </si>
+  <si>
+    <t>Centralized Action Management</t>
+  </si>
+  <si>
+    <t>GraFx Genie (AI powered Actions)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output to PDF with crop  marks </t>
+  </si>
+  <si>
+    <t>Import from Adobe® Illustrator®</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ❇️ Being developed</t>
   </si>
 </sst>
 </file>
@@ -976,2468 +982,2580 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26496501-D774-604E-8805-246C457AC686}">
-  <dimension ref="A1:D175"/>
+  <dimension ref="A1:D183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52.5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>191</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>161</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>169</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>170</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>128</v>
+        <v>10</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>169</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>128</v>
+        <v>89</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>1</v>
+        <v>137</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>177</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>128</v>
+        <v>13</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>179</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>128</v>
+        <v>140</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>128</v>
+        <v>141</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>138</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>1</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>175</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>176</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>128</v>
+        <v>34</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>128</v>
+        <v>171</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>128</v>
+        <v>35</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>128</v>
+        <v>90</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>181</v>
+        <v>36</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>47</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>128</v>
+        <v>38</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>171</v>
+        <v>39</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>48</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>49</v>
+        <v>177</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>175</v>
+        <v>41</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>1</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>1</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>1</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>178</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="C65" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>151</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>50</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>60</v>
+        <v>182</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>61</v>
+        <v>153</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>62</v>
+        <v>180</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>63</v>
+        <v>181</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>64</v>
+        <v>157</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>65</v>
+        <v>183</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>66</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>128</v>
+        <v>155</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>120</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>70</v>
+        <v>184</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>71</v>
+        <v>185</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>72</v>
+        <v>186</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>73</v>
+        <v>187</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>74</v>
+        <v>188</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>121</v>
+        <v>56</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>184</v>
+        <v>57</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>155</v>
+        <v>58</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>1</v>
+        <v>159</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>81</v>
+        <v>136</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>122</v>
+        <v>65</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>1</v>
+        <v>159</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>93</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>133</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>135</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>94</v>
+        <v>152</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>95</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>96</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>128</v>
+        <v>71</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>123</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>1</v>
+        <v>189</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>99</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>100</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>128</v>
+        <v>190</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>137</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>189</v>
+        <v>97</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>137</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>186</v>
+        <v>75</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>137</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>137</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>124</v>
+        <v>77</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>103</v>
+        <v>148</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>181</v>
+        <v>105</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>138</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D164" t="s">
-        <v>190</v>
+        <v>144</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>153</v>
+        <v>192</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>139</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>165</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>100</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>85</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>111</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>86</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>87</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>0</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>0</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[GraFx Studio] Feature update 20250228 (#468)
Co-authored-by: jeroencosyn <51122933+jeroencosyn@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
+++ b/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bram/Documents/GitHub.nosync/grafx-documentation/docs/CHILI-GraFx/applications/editor-comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5EB5E9-162D-DD4E-9C99-A5A20702AFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110B0A88-E9E0-FC42-81AB-DB657BCD4384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="760" windowWidth="28440" windowHeight="20840" xr2:uid="{BF9F8A34-DC7E-0549-A389-ADCA54F02979}"/>
   </bookViews>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26496501-D774-604E-8805-246C457AC686}">
   <dimension ref="A1:D183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1113,7 +1113,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>102</v>
@@ -1182,8 +1182,8 @@
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>0</v>
+      <c r="B14" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>102</v>
@@ -1687,7 +1687,7 @@
         <v>33</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>102</v>
@@ -3101,7 +3101,7 @@
         <v>75</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>102</v>
@@ -3282,8 +3282,8 @@
       <c r="A164" t="s">
         <v>167</v>
       </c>
-      <c r="B164" s="1" t="s">
-        <v>144</v>
+      <c r="B164" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
[GraFx Brand Kits] Initial Documentation (#551)
Co-authored-by: tbranko <tbranko@icloud.com>
Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
+++ b/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bram/Documents/GitHub.nosync/grafx-documentation/docs/CHILI-GraFx/applications/editor-comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110B0A88-E9E0-FC42-81AB-DB657BCD4384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6E59B1-D4D1-2E40-8540-8076927226FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="760" windowWidth="28440" windowHeight="20840" xr2:uid="{BF9F8A34-DC7E-0549-A389-ADCA54F02979}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="195">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -524,9 +524,6 @@
     <t>Support for Out-of-the-box self service</t>
   </si>
   <si>
-    <t>GraFx Studio: My Projects</t>
-  </si>
-  <si>
     <t>Connector Framework</t>
   </si>
   <si>
@@ -560,9 +557,6 @@
     <t xml:space="preserve">Border and fill settings </t>
   </si>
   <si>
-    <t>GraFx Studio: in Template Designer Workspace</t>
-  </si>
-  <si>
     <t>Support for Font Families management</t>
   </si>
   <si>
@@ -618,6 +612,15 @@
   </si>
   <si>
     <t xml:space="preserve"> ❇️ Being developed</t>
+  </si>
+  <si>
+    <t>Support for metadata mapping from PIM</t>
+  </si>
+  <si>
+    <t>Support for custom connectors (media &amp; data)</t>
+  </si>
+  <si>
+    <t>in Template Designer Workspace</t>
   </si>
 </sst>
 </file>
@@ -982,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26496501-D774-604E-8805-246C457AC686}">
-  <dimension ref="A1:D183"/>
+  <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -998,7 +1001,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>104</v>
@@ -1049,12 +1052,12 @@
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -1068,7 +1071,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>102</v>
@@ -1250,7 +1253,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>102</v>
@@ -1323,7 +1326,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>102</v>
@@ -1455,7 +1458,7 @@
         <v>102</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1561,7 +1564,7 @@
         <v>26</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>102</v>
@@ -1614,7 +1617,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>102</v>
@@ -1628,7 +1631,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>102</v>
@@ -1712,7 +1715,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>102</v>
@@ -1798,8 +1801,8 @@
       <c r="A58" t="s">
         <v>39</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>0</v>
+      <c r="B58" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>102</v>
@@ -1824,7 +1827,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>102</v>
@@ -1838,7 +1841,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>102</v>
@@ -1861,7 +1864,7 @@
         <v>102</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1875,7 +1878,7 @@
         <v>102</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1889,15 +1892,15 @@
         <v>102</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>102</v>
@@ -2020,7 +2023,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>102</v>
@@ -2121,7 +2124,7 @@
         <v>47</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>102</v>
@@ -2135,7 +2138,7 @@
         <v>48</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>102</v>
@@ -2188,7 +2191,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>0</v>
@@ -2216,7 +2219,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>0</v>
@@ -2230,7 +2233,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>0</v>
@@ -2258,7 +2261,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>102</v>
@@ -2356,7 +2359,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>0</v>
@@ -2370,7 +2373,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>0</v>
@@ -2384,7 +2387,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>0</v>
@@ -2398,7 +2401,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>0</v>
@@ -2412,7 +2415,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>0</v>
@@ -2583,7 +2586,7 @@
         <v>128</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>102</v>
@@ -3042,7 +3045,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>102</v>
@@ -3070,7 +3073,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>102</v>
@@ -3196,7 +3199,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>102</v>
@@ -3210,10 +3213,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>0</v>
@@ -3224,13 +3227,13 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>79</v>
+        <v>193</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>0</v>
@@ -3238,13 +3241,13 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>0</v>
@@ -3252,7 +3255,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>102</v>
@@ -3266,13 +3269,13 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>166</v>
+        <v>80</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>0</v>
@@ -3280,12 +3283,12 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>167</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C164" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C164" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3294,10 +3297,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>0</v>
@@ -3308,10 +3311,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>192</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>0</v>
+        <v>166</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>102</v>
@@ -3322,10 +3325,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>0</v>
@@ -3336,12 +3339,12 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>82</v>
+        <v>190</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C168" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C168" s="2" t="s">
         <v>102</v>
       </c>
       <c r="D168" s="1" t="s">
@@ -3350,13 +3353,13 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>191</v>
+        <v>99</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>0</v>
@@ -3364,9 +3367,9 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>83</v>
-      </c>
-      <c r="B170" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B170" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C170" s="1" t="s">
@@ -3378,7 +3381,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>121</v>
+        <v>189</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>102</v>
@@ -3392,9 +3395,9 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>122</v>
-      </c>
-      <c r="B172" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C172" s="1" t="s">
@@ -3406,13 +3409,13 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>0</v>
@@ -3420,13 +3423,13 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>0</v>
@@ -3434,13 +3437,13 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>0</v>
@@ -3448,13 +3451,13 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>0</v>
@@ -3462,13 +3465,13 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>0</v>
@@ -3476,10 +3479,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>85</v>
+        <v>164</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>102</v>
@@ -3490,10 +3493,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>0</v>
@@ -3504,7 +3507,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>102</v>
@@ -3518,13 +3521,13 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>0</v>
@@ -3532,13 +3535,13 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>0</v>
@@ -3546,15 +3549,43 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>193</v>
+        <v>102</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D183" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>0</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>0</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D185" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[GraFx-Studio] Photoshop Exporter (#558)
</commit_message>
<xml_diff>
--- a/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
+++ b/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10804"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bram/Documents/GitHub.nosync/grafx-documentation/docs/CHILI-GraFx/applications/editor-comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6E59B1-D4D1-2E40-8540-8076927226FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B379A68B-F5FE-EB4F-8A2B-33D8FC09C0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="760" windowWidth="28440" windowHeight="20840" xr2:uid="{BF9F8A34-DC7E-0549-A389-ADCA54F02979}"/>
+    <workbookView xWindow="9960" yWindow="760" windowWidth="34860" windowHeight="27640" xr2:uid="{BF9F8A34-DC7E-0549-A389-ADCA54F02979}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="203">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -621,6 +621,30 @@
   </si>
   <si>
     <t>in Template Designer Workspace</t>
+  </si>
+  <si>
+    <t>GraFx Studio supports several OTF [GPOS tables](/GraFx-Fonts/overview/supported-font-types/#supported-tables)</t>
+  </si>
+  <si>
+    <t>GPOS Single Adjust</t>
+  </si>
+  <si>
+    <t>GPOS Pair Adjust</t>
+  </si>
+  <si>
+    <t>GPOS Cursive</t>
+  </si>
+  <si>
+    <t>GPOS Mark-to-base</t>
+  </si>
+  <si>
+    <t>GPOS Mark-to-ligature</t>
+  </si>
+  <si>
+    <t>GPOS Mark-to-Mark</t>
+  </si>
+  <si>
+    <t>[Supported GPOS tables](/GraFx-Fonts/overview/supported-font-types/#supported-tables)</t>
   </si>
 </sst>
 </file>
@@ -985,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26496501-D774-604E-8805-246C457AC686}">
-  <dimension ref="A1:D185"/>
+  <dimension ref="A1:D191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1662,118 +1686,118 @@
         <v>31</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>0</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>196</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>105</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>197</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>198</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>36</v>
-      </c>
-      <c r="B55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -1785,10 +1809,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>38</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>102</v>
+        <v>34</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>102</v>
@@ -1799,9 +1823,9 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>39</v>
-      </c>
-      <c r="B58" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -1813,7 +1837,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>102</v>
@@ -1827,13 +1851,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>175</v>
+        <v>90</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>0</v>
@@ -1841,13 +1865,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>162</v>
-      </c>
-      <c r="B61" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>0</v>
@@ -1855,51 +1879,51 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>41</v>
-      </c>
-      <c r="B62" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>171</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>42</v>
-      </c>
-      <c r="B63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>171</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>139</v>
-      </c>
-      <c r="B64" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>171</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>176</v>
-      </c>
-      <c r="B65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C65" s="1" t="s">
@@ -1911,13 +1935,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>0</v>
@@ -1925,7 +1949,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>102</v>
@@ -1939,55 +1963,55 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>0</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>0</v>
+        <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>0</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>117</v>
+        <v>176</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>0</v>
@@ -1995,10 +2019,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>0</v>
@@ -2009,7 +2033,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>102</v>
@@ -2023,7 +2047,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>177</v>
+        <v>114</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>102</v>
@@ -2037,9 +2061,9 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>120</v>
-      </c>
-      <c r="B75" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -2051,10 +2075,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>0</v>
@@ -2065,13 +2089,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>0</v>
@@ -2079,13 +2103,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>0</v>
@@ -2093,13 +2117,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>0</v>
@@ -2107,13 +2131,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>0</v>
@@ -2121,13 +2145,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>47</v>
-      </c>
-      <c r="B81" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>0</v>
@@ -2135,13 +2159,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>0</v>
@@ -2149,7 +2173,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>102</v>
@@ -2163,13 +2187,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>0</v>
@@ -2177,7 +2201,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>102</v>
@@ -2191,7 +2215,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>180</v>
+        <v>46</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>0</v>
@@ -2205,7 +2229,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>153</v>
+        <v>47</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>102</v>
@@ -2219,10 +2243,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>178</v>
+        <v>48</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>102</v>
@@ -2233,10 +2257,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>179</v>
+        <v>49</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>102</v>
@@ -2247,13 +2271,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>157</v>
+        <v>92</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>102</v>
+        <v>0</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>0</v>
@@ -2261,7 +2285,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>102</v>
@@ -2275,12 +2299,12 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>155</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C92" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2289,7 +2313,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>102</v>
@@ -2303,10 +2327,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>50</v>
+        <v>178</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>102</v>
@@ -2317,10 +2341,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>154</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>102</v>
+        <v>179</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>102</v>
@@ -2331,12 +2355,12 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>51</v>
+        <v>157</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="2" t="s">
         <v>102</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2345,10 +2369,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>52</v>
+        <v>181</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>102</v>
@@ -2359,12 +2383,12 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>182</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C98" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>102</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2373,10 +2397,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>102</v>
@@ -2387,10 +2411,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>184</v>
+        <v>50</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>102</v>
@@ -2401,10 +2425,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>185</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>0</v>
+        <v>154</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>102</v>
@@ -2415,10 +2439,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>186</v>
+        <v>51</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>102</v>
@@ -2429,13 +2453,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>0</v>
@@ -2443,7 +2467,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>53</v>
+        <v>182</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>0</v>
@@ -2457,13 +2481,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>0</v>
@@ -2471,7 +2495,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>54</v>
+        <v>184</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>0</v>
@@ -2485,7 +2509,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>0</v>
@@ -2499,7 +2523,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>56</v>
+        <v>186</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>0</v>
@@ -2513,13 +2537,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>0</v>
@@ -2527,7 +2551,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>0</v>
@@ -2541,7 +2565,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>0</v>
@@ -2555,10 +2579,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>145</v>
+        <v>54</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>102</v>
@@ -2569,10 +2593,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>124</v>
+        <v>55</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>102</v>
@@ -2583,10 +2607,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>102</v>
@@ -2597,7 +2621,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>0</v>
@@ -2611,7 +2635,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>126</v>
+        <v>58</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>0</v>
@@ -2625,21 +2649,21 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>159</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>102</v>
@@ -2653,7 +2677,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>102</v>
@@ -2667,7 +2691,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>102</v>
@@ -2681,10 +2705,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>102</v>
@@ -2695,10 +2719,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>102</v>
@@ -2709,24 +2733,24 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>0</v>
+        <v>159</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>102</v>
@@ -2737,10 +2761,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>102</v>
@@ -2751,7 +2775,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>102</v>
@@ -2765,7 +2789,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>102</v>
@@ -2779,7 +2803,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>102</v>
@@ -2793,10 +2817,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>102</v>
@@ -2807,10 +2831,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>102</v>
@@ -2821,10 +2845,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>64</v>
+        <v>136</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>102</v>
@@ -2835,7 +2859,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>102</v>
@@ -2844,12 +2868,12 @@
         <v>102</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>159</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>102</v>
@@ -2863,13 +2887,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>0</v>
@@ -2877,7 +2901,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>102</v>
@@ -2891,7 +2915,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>102</v>
@@ -2905,10 +2929,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>102</v>
@@ -2919,23 +2943,23 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>146</v>
+        <v>65</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>106</v>
-      </c>
-      <c r="B139" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C139" s="1" t="s">
@@ -2947,13 +2971,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>107</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>0</v>
@@ -2961,13 +2985,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>151</v>
-      </c>
-      <c r="B141" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>0</v>
@@ -2975,13 +2999,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>152</v>
-      </c>
-      <c r="B142" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>0</v>
@@ -2989,9 +3013,9 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>70</v>
-      </c>
-      <c r="B143" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C143" s="1" t="s">
@@ -3003,21 +3027,21 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>71</v>
+        <v>146</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>102</v>
@@ -3026,12 +3050,12 @@
         <v>102</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>108</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>102</v>
@@ -3045,7 +3069,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>102</v>
@@ -3059,13 +3083,13 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>0</v>
@@ -3073,13 +3097,13 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>188</v>
+        <v>70</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>0</v>
@@ -3087,13 +3111,13 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>0</v>
@@ -3101,23 +3125,23 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>75</v>
-      </c>
-      <c r="B151" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>0</v>
+        <v>108</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>76</v>
-      </c>
-      <c r="B152" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C152" s="1" t="s">
@@ -3129,41 +3153,41 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>149</v>
-      </c>
-      <c r="B153" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>147</v>
-      </c>
-      <c r="B154" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>77</v>
-      </c>
-      <c r="B155" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>0</v>
@@ -3171,21 +3195,21 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>148</v>
+        <v>97</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>102</v>
@@ -3199,13 +3223,13 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>192</v>
+        <v>76</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>0</v>
@@ -3213,41 +3237,41 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>0</v>
+        <v>109</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>193</v>
+        <v>147</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>0</v>
+        <v>109</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>0</v>
@@ -3255,21 +3279,21 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>102</v>
@@ -3283,13 +3307,13 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>81</v>
+        <v>192</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>0</v>
@@ -3297,10 +3321,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>0</v>
@@ -3311,13 +3335,13 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>166</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>102</v>
+        <v>193</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>0</v>
@@ -3325,10 +3349,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>167</v>
+        <v>98</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>0</v>
@@ -3339,12 +3363,12 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>190</v>
+        <v>79</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C168" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C168" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D168" s="1" t="s">
@@ -3353,13 +3377,13 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>0</v>
@@ -3367,7 +3391,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>102</v>
@@ -3381,13 +3405,13 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>0</v>
@@ -3395,12 +3419,12 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C172" s="1" t="s">
+      <c r="C172" s="2" t="s">
         <v>102</v>
       </c>
       <c r="D172" s="1" t="s">
@@ -3409,13 +3433,13 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>121</v>
-      </c>
-      <c r="B173" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>0</v>
@@ -3423,12 +3447,12 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C174" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C174" s="2" t="s">
         <v>102</v>
       </c>
       <c r="D174" s="1" t="s">
@@ -3437,10 +3461,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>0</v>
@@ -3451,13 +3475,13 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>0</v>
@@ -3465,10 +3489,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>84</v>
+        <v>189</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>102</v>
@@ -3479,10 +3503,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>164</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>102</v>
@@ -3493,13 +3517,13 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>0</v>
@@ -3507,7 +3531,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>102</v>
@@ -3521,7 +3545,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>102</v>
@@ -3535,13 +3559,13 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>0</v>
@@ -3549,10 +3573,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>102</v>
@@ -3563,13 +3587,13 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>0</v>
@@ -3577,15 +3601,99 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="B185" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>85</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>111</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>86</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>87</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>0</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>0</v>
+      </c>
+      <c r="B191" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C185" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D185" s="1" t="s">
+      <c r="C191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D191" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Documentation] Updated several videos (#601)
</commit_message>
<xml_diff>
--- a/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
+++ b/docs/CHILI-GraFx/applications/editor-comparison/features.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10804"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bram/Documents/GitHub.nosync/grafx-documentation/docs/CHILI-GraFx/applications/editor-comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B379A68B-F5FE-EB4F-8A2B-33D8FC09C0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CAE5D7-F793-3340-9F95-F9E51EFC91AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="760" windowWidth="34860" windowHeight="27640" xr2:uid="{BF9F8A34-DC7E-0549-A389-ADCA54F02979}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="205">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -185,9 +185,6 @@
     <t xml:space="preserve">Support for gradients </t>
   </si>
   <si>
-    <t xml:space="preserve">Custom color swatches </t>
-  </si>
-  <si>
     <t xml:space="preserve">Support for EAN13 </t>
   </si>
   <si>
@@ -645,6 +642,15 @@
   </si>
   <si>
     <t>[Supported GPOS tables](/GraFx-Fonts/overview/supported-font-types/#supported-tables)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom colors </t>
+  </si>
+  <si>
+    <t>Will be covered by Components in GraFx Studio</t>
+  </si>
+  <si>
+    <t>Import from Figma</t>
   </si>
 </sst>
 </file>
@@ -1009,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26496501-D774-604E-8805-246C457AC686}">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:D192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1025,35 +1031,35 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -1067,10 +1073,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -1081,7 +1087,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -1095,13 +1101,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>0</v>
@@ -1109,10 +1115,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
@@ -1126,13 +1132,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1140,13 +1146,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1154,13 +1160,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1171,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>0</v>
@@ -1185,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>0</v>
@@ -1199,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
@@ -1210,10 +1216,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>0</v>
@@ -1227,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>0</v>
@@ -1241,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>0</v>
@@ -1252,10 +1258,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>0</v>
@@ -1263,7 +1269,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>0</v>
@@ -1277,13 +1283,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>0</v>
@@ -1297,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>0</v>
@@ -1305,13 +1311,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>0</v>
@@ -1325,10 +1331,10 @@
         <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1336,80 +1342,80 @@
         <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>144</v>
+      <c r="B24" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>0</v>
@@ -1420,10 +1426,10 @@
         <v>15</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>0</v>
@@ -1437,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>0</v>
@@ -1448,10 +1454,10 @@
         <v>17</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>0</v>
@@ -1459,7 +1465,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>0</v>
@@ -1476,13 +1482,13 @@
         <v>18</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1493,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>0</v>
@@ -1504,10 +1510,10 @@
         <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>0</v>
@@ -1518,10 +1524,10 @@
         <v>21</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>0</v>
@@ -1535,7 +1541,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>0</v>
@@ -1546,10 +1552,10 @@
         <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>0</v>
@@ -1560,10 +1566,10 @@
         <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>0</v>
@@ -1574,10 +1580,10 @@
         <v>25</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>0</v>
@@ -1588,10 +1594,10 @@
         <v>26</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>0</v>
@@ -1605,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>0</v>
@@ -1616,10 +1622,10 @@
         <v>28</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>0</v>
@@ -1630,10 +1636,10 @@
         <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>0</v>
@@ -1641,10 +1647,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
@@ -1655,10 +1661,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -1672,10 +1678,10 @@
         <v>30</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>0</v>
@@ -1686,97 +1692,97 @@
         <v>31</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>200</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1784,13 +1790,13 @@
         <v>32</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1798,10 +1804,10 @@
         <v>33</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>0</v>
@@ -1815,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>0</v>
@@ -1823,13 +1829,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>0</v>
@@ -1840,10 +1846,10 @@
         <v>35</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>0</v>
@@ -1851,7 +1857,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>0</v>
@@ -1868,10 +1874,10 @@
         <v>36</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>0</v>
@@ -1882,10 +1888,10 @@
         <v>37</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>0</v>
@@ -1896,10 +1902,10 @@
         <v>38</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>0</v>
@@ -1910,10 +1916,10 @@
         <v>39</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>0</v>
@@ -1924,10 +1930,10 @@
         <v>40</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>0</v>
@@ -1935,13 +1941,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>0</v>
@@ -1949,10 +1955,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>0</v>
@@ -1966,13 +1972,13 @@
         <v>41</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1980,38 +1986,38 @@
         <v>42</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>0</v>
@@ -2019,7 +2025,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>0</v>
@@ -2033,10 +2039,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>0</v>
@@ -2047,10 +2053,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>0</v>
@@ -2061,10 +2067,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>0</v>
@@ -2075,10 +2081,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>0</v>
@@ -2089,10 +2095,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>0</v>
@@ -2103,10 +2109,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>0</v>
@@ -2117,10 +2123,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>0</v>
@@ -2131,10 +2137,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>0</v>
@@ -2145,10 +2151,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>0</v>
@@ -2159,7 +2165,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>0</v>
@@ -2176,10 +2182,10 @@
         <v>43</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>0</v>
@@ -2190,10 +2196,10 @@
         <v>44</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>0</v>
@@ -2204,10 +2210,10 @@
         <v>45</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>0</v>
@@ -2221,7 +2227,7 @@
         <v>0</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>0</v>
@@ -2232,10 +2238,10 @@
         <v>47</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>0</v>
@@ -2246,10 +2252,10 @@
         <v>48</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>0</v>
@@ -2257,13 +2263,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>49</v>
+        <v>202</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>0</v>
@@ -2271,7 +2277,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>0</v>
@@ -2285,13 +2291,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>0</v>
@@ -2299,13 +2305,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>0</v>
@@ -2313,13 +2319,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>0</v>
@@ -2327,13 +2333,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>0</v>
@@ -2341,13 +2347,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>0</v>
@@ -2355,13 +2361,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>0</v>
@@ -2369,13 +2375,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>0</v>
@@ -2383,13 +2389,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>0</v>
@@ -2397,13 +2403,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>0</v>
@@ -2411,13 +2417,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>0</v>
@@ -2425,13 +2431,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>0</v>
@@ -2439,13 +2445,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>0</v>
@@ -2453,13 +2459,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>0</v>
@@ -2467,13 +2473,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>0</v>
@@ -2481,13 +2487,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>0</v>
@@ -2495,13 +2501,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>0</v>
@@ -2509,13 +2515,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>0</v>
@@ -2523,13 +2529,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>0</v>
@@ -2537,7 +2543,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>0</v>
@@ -2551,13 +2557,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>0</v>
@@ -2565,7 +2571,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>0</v>
@@ -2579,13 +2585,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>0</v>
@@ -2593,13 +2599,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>0</v>
@@ -2607,13 +2613,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>0</v>
@@ -2621,13 +2627,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>0</v>
@@ -2635,13 +2641,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>0</v>
@@ -2649,7 +2655,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>0</v>
@@ -2663,13 +2669,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>0</v>
@@ -2677,13 +2683,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>0</v>
@@ -2691,13 +2697,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>0</v>
@@ -2705,13 +2711,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>0</v>
@@ -2719,13 +2725,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>0</v>
@@ -2733,27 +2739,27 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>0</v>
@@ -2761,13 +2767,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>0</v>
@@ -2775,13 +2781,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>0</v>
@@ -2789,13 +2795,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>0</v>
@@ -2803,13 +2809,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>0</v>
@@ -2817,13 +2823,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>0</v>
@@ -2831,13 +2837,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>0</v>
@@ -2845,13 +2851,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>0</v>
@@ -2859,13 +2865,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>0</v>
@@ -2873,13 +2879,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>0</v>
@@ -2887,13 +2893,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>0</v>
@@ -2901,13 +2907,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>0</v>
@@ -2915,13 +2921,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>0</v>
@@ -2929,13 +2935,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>0</v>
@@ -2943,27 +2949,27 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>0</v>
@@ -2971,7 +2977,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>0</v>
@@ -2985,13 +2991,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>0</v>
@@ -2999,13 +3005,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>0</v>
@@ -3013,13 +3019,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>0</v>
@@ -3027,27 +3033,27 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>0</v>
@@ -3055,13 +3061,13 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>0</v>
@@ -3069,10 +3075,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>0</v>
@@ -3083,10 +3089,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>0</v>
@@ -3097,13 +3103,13 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>0</v>
@@ -3111,41 +3117,41 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>0</v>
+        <v>203</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>0</v>
@@ -3153,10 +3159,10 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>0</v>
@@ -3167,13 +3173,13 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>0</v>
@@ -3181,10 +3187,10 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>0</v>
@@ -3195,7 +3201,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>0</v>
@@ -3209,13 +3215,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>0</v>
@@ -3223,13 +3229,13 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>0</v>
@@ -3237,41 +3243,41 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>0</v>
@@ -3279,27 +3285,27 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>0</v>
@@ -3307,10 +3313,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>0</v>
@@ -3321,10 +3327,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>0</v>
@@ -3335,10 +3341,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>0</v>
@@ -3349,7 +3355,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>0</v>
@@ -3363,13 +3369,13 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>0</v>
@@ -3377,13 +3383,13 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>0</v>
@@ -3391,13 +3397,13 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>0</v>
@@ -3405,7 +3411,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>0</v>
@@ -3419,13 +3425,13 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>0</v>
@@ -3433,10 +3439,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>0</v>
@@ -3447,13 +3453,13 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>0</v>
@@ -3461,12 +3467,12 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>99</v>
+        <v>204</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C175" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C175" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D175" s="1" t="s">
@@ -3475,13 +3481,13 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>0</v>
@@ -3489,13 +3495,13 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>189</v>
+        <v>81</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>0</v>
@@ -3503,13 +3509,13 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>83</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>102</v>
+        <v>188</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>0</v>
@@ -3517,13 +3523,13 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>121</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>102</v>
+        <v>82</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>0</v>
@@ -3531,13 +3537,13 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>0</v>
@@ -3545,13 +3551,13 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>0</v>
@@ -3559,10 +3565,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>0</v>
@@ -3573,13 +3579,13 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>0</v>
@@ -3587,13 +3593,13 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>164</v>
+        <v>83</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>0</v>
@@ -3601,13 +3607,13 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>0</v>
@@ -3615,13 +3621,13 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>0</v>
@@ -3629,13 +3635,13 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>0</v>
@@ -3643,13 +3649,13 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>0</v>
@@ -3657,13 +3663,13 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>0</v>
@@ -3671,13 +3677,13 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>0</v>
@@ -3688,12 +3694,26 @@
         <v>0</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>191</v>
+        <v>0</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D191" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>0</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D192" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>